<commit_message>
Updated field description spreadsheet
</commit_message>
<xml_diff>
--- a/Field descriptions Sherwin et al.xlsx
+++ b/Field descriptions Sherwin et al.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Backupworthy/Fall_2019/Gas/GTI/ACS Omega transfer/What we submitted/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{076D6097-AA88-4C48-8B82-64FB8A97DFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFFBAD6-13A9-034E-BA1D-876451599810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20700" windowHeight="13920" xr2:uid="{D925B7E5-E7D7-2849-A1B5-D356D0F0D742}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Service datatypes" sheetId="1" r:id="rId1"/>
     <sheet name="Leak datatypes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="282">
   <si>
     <t>objectid</t>
   </si>
@@ -140,9 +140,6 @@
   </si>
   <si>
     <t>corrodibleriserindicator</t>
-  </si>
-  <si>
-    <t>pgeremoteunitnumber</t>
   </si>
   <si>
     <t>remoteinstallationdate</t>
@@ -1252,13 +1249,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{237E4145-A836-5B4E-A98B-8DF319D62F79}">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37:C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1269,17 +1266,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1287,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1295,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1303,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1311,7 +1308,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1319,7 +1316,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1327,10 +1324,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1338,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1346,7 +1343,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1354,10 +1351,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1365,7 +1362,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,7 +1370,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1381,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1389,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1397,7 +1394,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1405,7 +1402,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1413,7 +1410,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1421,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1429,10 +1426,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1440,7 +1437,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1448,7 +1445,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1456,7 +1453,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1464,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1472,7 +1469,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1480,7 +1477,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1488,7 +1485,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1496,7 +1493,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1504,7 +1501,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1512,7 +1509,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1520,7 +1517,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1528,7 +1525,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1536,7 +1533,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1544,7 +1541,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1552,7 +1549,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1560,7 +1557,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1568,7 +1565,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1576,7 +1573,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +1581,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1592,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1600,7 +1597,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1608,7 +1605,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1616,7 +1613,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1624,7 +1621,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1634,16 +1634,13 @@
       <c r="B44" t="s">
         <v>121</v>
       </c>
-      <c r="C44" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1659,7 +1656,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -1667,7 +1664,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -1683,7 +1680,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1691,7 +1688,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
@@ -1699,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1707,7 +1704,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -1715,7 +1712,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
@@ -1723,7 +1720,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -1731,7 +1728,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -1739,7 +1736,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
@@ -1747,7 +1744,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -1755,7 +1752,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
@@ -1763,7 +1760,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
@@ -1771,7 +1768,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
@@ -1779,7 +1776,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
@@ -1787,7 +1784,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -1795,7 +1792,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1803,7 +1800,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
@@ -1811,7 +1808,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -1827,7 +1824,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
@@ -1835,7 +1832,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1851,7 +1848,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -1859,7 +1856,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -1875,7 +1872,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
@@ -1883,7 +1880,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1891,14 +1888,14 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="1" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1907,7 +1904,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
@@ -1915,7 +1912,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
@@ -1923,7 +1920,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1931,7 +1928,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
@@ -1939,7 +1936,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
@@ -1947,22 +1944,22 @@
         <v>81</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>82</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>122</v>
+      <c r="B84" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="1" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1971,7 +1968,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
@@ -1979,7 +1976,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
@@ -1987,7 +1984,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
@@ -1995,7 +1992,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
@@ -2003,7 +2000,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -2011,15 +2008,15 @@
         <v>89</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>122</v>
+      <c r="B92" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -2027,22 +2024,22 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
-        <v>122</v>
+      <c r="B94" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>122</v>
       </c>
     </row>
@@ -2050,16 +2047,16 @@
       <c r="A96" t="s">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
-        <v>123</v>
+      <c r="B96" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>122</v>
+      <c r="B97" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2074,8 +2071,8 @@
       <c r="A99" t="s">
         <v>97</v>
       </c>
-      <c r="B99" t="s">
-        <v>122</v>
+      <c r="B99" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2083,7 +2080,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,8 +2095,8 @@
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>123</v>
+      <c r="B102" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2107,7 +2104,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2115,7 +2112,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
@@ -2123,7 +2120,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2131,23 +2128,26 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B107" t="s">
-        <v>122</v>
+      <c r="B107" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108" s="1" t="s">
-        <v>122</v>
+      <c r="B108" t="s">
+        <v>121</v>
+      </c>
+      <c r="C108" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2155,10 +2155,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>122</v>
-      </c>
-      <c r="C109" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2166,7 +2163,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2174,7 +2171,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2182,7 +2179,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
@@ -2190,7 +2187,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
@@ -2198,7 +2195,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -2206,7 +2203,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
@@ -2222,7 +2219,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
@@ -2230,7 +2227,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
@@ -2238,15 +2235,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>118</v>
-      </c>
-      <c r="B120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2271,16 +2260,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2288,269 +2277,269 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B33" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -2558,10 +2547,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -2569,66 +2558,66 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
@@ -2636,938 +2625,938 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B154" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>